<commit_message>
xuhonglin_order_1.xls Signed-off-by: twtcom001 <twtcom001@sina.com>
</commit_message>
<xml_diff>
--- a/统计清单/中英文对照.xlsx
+++ b/统计清单/中英文对照.xlsx
@@ -12,7 +12,7 @@
     <sheet name="合并名称集合" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1560,10 +1560,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mammillaria camptotricha cv. Bru  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gymnocalycium prochazkianum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2595,6 +2591,10 @@
   </si>
   <si>
     <t>Ariocarpus retusus var. furfuraceus cv. Brebituberosus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gymnocalycium prochazkianum</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3313,8 +3313,8 @@
   <dimension ref="A1:F234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B160" sqref="B160"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3342,7 +3342,7 @@
         <v>279</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>45</v>
@@ -3364,13 +3364,13 @@
         <v>367</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="16" t="s">
         <v>605</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3389,10 +3389,10 @@
         <v>367</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -3411,10 +3411,10 @@
         <v>367</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>603</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -3425,10 +3425,10 @@
         <v>367</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3436,10 +3436,10 @@
         <v>367</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -3450,7 +3450,7 @@
         <v>375</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3458,7 +3458,7 @@
         <v>367</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>377</v>
@@ -3469,10 +3469,10 @@
         <v>367</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -3483,7 +3483,7 @@
         <v>376</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3502,10 +3502,10 @@
         <v>367</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>600</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>601</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -3516,10 +3516,10 @@
         <v>367</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>623</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -3527,13 +3527,13 @@
         <v>367</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>618</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -3544,7 +3544,7 @@
         <v>371</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
@@ -3555,10 +3555,10 @@
         <v>367</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -3704,7 +3704,7 @@
         <v>334</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>15</v>
@@ -3748,10 +3748,10 @@
         <v>334</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -3759,10 +3759,10 @@
         <v>334</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -3770,10 +3770,10 @@
         <v>334</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -3781,10 +3781,10 @@
         <v>334</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -3792,10 +3792,10 @@
         <v>334</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -3803,10 +3803,10 @@
         <v>334</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -3814,10 +3814,10 @@
         <v>334</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -3825,10 +3825,10 @@
         <v>334</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -3836,10 +3836,10 @@
         <v>334</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -3847,10 +3847,10 @@
         <v>334</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -3880,10 +3880,10 @@
         <v>334</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -3891,7 +3891,7 @@
         <v>334</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>23</v>
@@ -3905,7 +3905,7 @@
         <v>22</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -3924,7 +3924,7 @@
         <v>334</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>21</v>
@@ -3935,7 +3935,7 @@
         <v>334</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>24</v>
@@ -3946,10 +3946,10 @@
         <v>334</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -3957,10 +3957,10 @@
         <v>334</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -3968,10 +3968,10 @@
         <v>334</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -3979,10 +3979,10 @@
         <v>334</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>576</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -3990,10 +3990,10 @@
         <v>334</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -4001,10 +4001,10 @@
         <v>334</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -4012,10 +4012,10 @@
         <v>334</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -4023,10 +4023,10 @@
         <v>334</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -4045,10 +4045,10 @@
         <v>334</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -4056,10 +4056,10 @@
         <v>334</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -4067,10 +4067,10 @@
         <v>334</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -4100,10 +4100,10 @@
         <v>333</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>469</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>470</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
@@ -4114,7 +4114,7 @@
         <v>338</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>340</v>
@@ -4122,13 +4122,13 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B69" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="C69" s="15" t="s">
         <v>405</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>406</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
@@ -4136,27 +4136,27 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C70" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="F71" s="16" t="s">
         <v>484</v>
-      </c>
-      <c r="F71" s="16" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -4200,10 +4200,10 @@
         <v>328</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -4211,10 +4211,10 @@
         <v>328</v>
       </c>
       <c r="B76" s="20" t="s">
+        <v>536</v>
+      </c>
+      <c r="C76" s="21" t="s">
         <v>537</v>
-      </c>
-      <c r="C76" s="21" t="s">
-        <v>538</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="21"/>
@@ -4225,10 +4225,10 @@
         <v>328</v>
       </c>
       <c r="B77" s="20" t="s">
+        <v>538</v>
+      </c>
+      <c r="C77" s="21" t="s">
         <v>539</v>
-      </c>
-      <c r="C77" s="21" t="s">
-        <v>540</v>
       </c>
       <c r="D77" s="21"/>
       <c r="E77" s="21"/>
@@ -4252,7 +4252,7 @@
         <v>330</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>40</v>
@@ -4307,24 +4307,24 @@
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B85" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="C85" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="F85" s="16" t="s">
         <v>492</v>
-      </c>
-      <c r="F85" s="16" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -4346,10 +4346,10 @@
         <v>256</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -4379,7 +4379,7 @@
         <v>256</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>168</v>
@@ -4401,10 +4401,10 @@
         <v>257</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
@@ -4500,13 +4500,13 @@
         <v>257</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="F100" s="16" t="s">
         <v>481</v>
-      </c>
-      <c r="F100" s="16" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="33" x14ac:dyDescent="0.3">
@@ -4514,15 +4514,15 @@
         <v>257</v>
       </c>
       <c r="B101" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="C101" s="15" t="s">
         <v>436</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>437</v>
       </c>
       <c r="D101" s="15"/>
       <c r="E101" s="15"/>
       <c r="F101" s="16" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -4549,7 +4549,7 @@
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
       <c r="F103" s="16" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -4704,10 +4704,10 @@
         <v>257</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D116" s="15"/>
       <c r="E116" s="15">
@@ -4773,10 +4773,10 @@
         <v>257</v>
       </c>
       <c r="B121" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C121" s="16" t="s">
         <v>440</v>
-      </c>
-      <c r="C121" s="16" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="66" x14ac:dyDescent="0.3">
@@ -4784,15 +4784,15 @@
         <v>257</v>
       </c>
       <c r="B122" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C122" s="16" t="s">
         <v>438</v>
-      </c>
-      <c r="C122" s="16" t="s">
-        <v>439</v>
       </c>
       <c r="D122" s="15"/>
       <c r="E122" s="15"/>
       <c r="F122" s="16" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -4808,18 +4808,18 @@
     </row>
     <row r="124" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A124" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="C124" s="15" t="s">
         <v>476</v>
-      </c>
-      <c r="B124" s="14" t="s">
-        <v>475</v>
-      </c>
-      <c r="C124" s="15" t="s">
-        <v>477</v>
       </c>
       <c r="D124" s="15"/>
       <c r="E124" s="15"/>
       <c r="F124" s="16" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -4827,10 +4827,10 @@
         <v>335</v>
       </c>
       <c r="B125" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -4838,10 +4838,10 @@
         <v>335</v>
       </c>
       <c r="B126" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -4849,10 +4849,10 @@
         <v>335</v>
       </c>
       <c r="B127" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -4860,10 +4860,10 @@
         <v>335</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -4885,13 +4885,13 @@
         <v>335</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F130" s="16" t="s">
         <v>424</v>
-      </c>
-      <c r="F130" s="16" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -4899,13 +4899,13 @@
         <v>335</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C131" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F131" s="16" t="s">
         <v>426</v>
-      </c>
-      <c r="F131" s="16" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -4913,10 +4913,10 @@
         <v>335</v>
       </c>
       <c r="B132" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -4957,13 +4957,13 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C136" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="15"/>
@@ -4971,62 +4971,62 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B137" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B139" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C139" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>249</v>
@@ -5037,7 +5037,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>247</v>
@@ -5048,7 +5048,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>199</v>
@@ -5059,21 +5059,21 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B145" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="B145" s="3" t="s">
+      <c r="C145" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>119</v>
@@ -5081,10 +5081,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>396</v>
+        <v>625</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>164</v>
@@ -5092,7 +5092,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>200</v>
@@ -5114,7 +5114,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>213</v>
@@ -5132,7 +5132,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>215</v>
@@ -5149,7 +5149,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>217</v>
@@ -5166,7 +5166,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>219</v>
@@ -5183,7 +5183,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>221</v>
@@ -5200,10 +5200,10 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>237</v>
@@ -5218,7 +5218,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>227</v>
@@ -5235,7 +5235,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>223</v>
@@ -5252,7 +5252,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>232</v>
@@ -5269,7 +5269,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>229</v>
@@ -5286,7 +5286,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>233</v>
@@ -5295,7 +5295,7 @@
         <v>237</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F160" s="16" t="s">
         <v>238</v>
@@ -5303,7 +5303,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>225</v>
@@ -5580,24 +5580,24 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B185" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="B185" s="3" t="s">
-        <v>430</v>
-      </c>
       <c r="C185" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
@@ -5613,13 +5613,13 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
@@ -5697,13 +5697,13 @@
         <v>184</v>
       </c>
       <c r="B193" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="F193" s="16" t="s">
         <v>472</v>
-      </c>
-      <c r="C193" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="F193" s="16" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
@@ -5719,13 +5719,13 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D195" s="15"/>
       <c r="E195" s="15"/>
@@ -5733,13 +5733,13 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B196" s="14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C196" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D196" s="15"/>
       <c r="E196" s="15"/>
@@ -5747,13 +5747,13 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B197" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C197" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
@@ -5761,13 +5761,13 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C198" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
@@ -5775,13 +5775,13 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B199" s="14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C199" s="15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D199" s="15"/>
       <c r="E199" s="15"/>
@@ -5789,13 +5789,13 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B200" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="C200" s="15" t="s">
         <v>466</v>
-      </c>
-      <c r="C200" s="15" t="s">
-        <v>467</v>
       </c>
       <c r="D200" s="15"/>
       <c r="E200" s="15"/>
@@ -5803,13 +5803,13 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B201" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="C201" s="15" t="s">
         <v>464</v>
-      </c>
-      <c r="C201" s="15" t="s">
-        <v>465</v>
       </c>
       <c r="D201" s="15"/>
       <c r="E201" s="15"/>
@@ -5817,13 +5817,13 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="B202" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="C202" s="15" t="s">
         <v>462</v>
-      </c>
-      <c r="B202" s="14" t="s">
-        <v>460</v>
-      </c>
-      <c r="C202" s="15" t="s">
-        <v>463</v>
       </c>
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
@@ -5831,18 +5831,18 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" s="20" t="s">
+        <v>532</v>
+      </c>
+      <c r="B203" s="20" t="s">
+        <v>535</v>
+      </c>
+      <c r="C203" s="21" t="s">
         <v>533</v>
-      </c>
-      <c r="B203" s="20" t="s">
-        <v>536</v>
-      </c>
-      <c r="C203" s="21" t="s">
-        <v>534</v>
       </c>
       <c r="D203" s="21"/>
       <c r="E203" s="21"/>
       <c r="F203" s="22" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
@@ -5927,7 +5927,7 @@
         <v>345</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>346</v>
@@ -5963,7 +5963,7 @@
         <v>341</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C214" s="9" t="s">
         <v>309</v>
@@ -6254,7 +6254,7 @@
         <v>341</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C233" s="8" t="s">
         <v>311</v>
@@ -6319,10 +6319,10 @@
     </row>
     <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>125</v>
@@ -6330,10 +6330,10 @@
     </row>
     <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>126</v>
@@ -6341,10 +6341,10 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>127</v>
@@ -6352,10 +6352,10 @@
     </row>
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>128</v>
@@ -6363,10 +6363,10 @@
     </row>
     <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>129</v>
@@ -6374,10 +6374,10 @@
     </row>
     <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>130</v>
@@ -6385,10 +6385,10 @@
     </row>
     <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>131</v>
@@ -6396,10 +6396,10 @@
     </row>
     <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>132</v>
@@ -6407,10 +6407,10 @@
     </row>
     <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>133</v>
@@ -6418,10 +6418,10 @@
     </row>
     <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>134</v>
@@ -6429,10 +6429,10 @@
     </row>
     <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>135</v>
@@ -6440,10 +6440,10 @@
     </row>
     <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>136</v>
@@ -6451,21 +6451,21 @@
     </row>
     <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>517</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>519</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>137</v>
@@ -6473,10 +6473,10 @@
     </row>
     <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>138</v>
@@ -6484,10 +6484,10 @@
     </row>
     <row r="17" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>139</v>
@@ -6495,10 +6495,10 @@
     </row>
     <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>139</v>
@@ -6506,10 +6506,10 @@
     </row>
     <row r="19" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>140</v>
@@ -6517,10 +6517,10 @@
     </row>
     <row r="20" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>141</v>
@@ -6528,10 +6528,10 @@
     </row>
     <row r="21" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>142</v>
@@ -6539,10 +6539,10 @@
     </row>
     <row r="22" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>143</v>
@@ -6550,10 +6550,10 @@
     </row>
     <row r="23" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>144</v>
@@ -6561,10 +6561,10 @@
     </row>
     <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>145</v>
@@ -6572,10 +6572,10 @@
     </row>
     <row r="25" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>146</v>
@@ -6583,10 +6583,10 @@
     </row>
     <row r="26" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>380</v>
@@ -6594,10 +6594,10 @@
     </row>
     <row r="27" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>147</v>
@@ -6691,34 +6691,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>595</v>
+      </c>
+      <c r="B4" t="s">
         <v>596</v>
-      </c>
-      <c r="B4" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>

</xml_diff>